<commit_message>
Aggiornato schematico e lista parti per sostituire C9 con 100nF Con 10nF la tensione di reference potrebbe essere instabile
</commit_message>
<xml_diff>
--- a/ESECUTIVI/LP22-310-0.xlsx
+++ b/ESECUTIVI/LP22-310-0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Utenti\00.Lavori in corso\METALTRONICA\22-310-0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Documents\Data\Progetti-GIT\HW\PCB-22-310\ESECUTIVI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F98C10F-F5FD-4EBD-B0A3-F4552351BFF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110ADD03-72A8-4D11-A96A-B316F97235F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
+    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="22-310-0" sheetId="1" r:id="rId1"/>
@@ -73,9 +73,6 @@
     <t>MLCC, X7R, 100V 0805</t>
   </si>
   <si>
-    <t>C2,C3,C4,C6,C8,C11,C15,C16</t>
-  </si>
-  <si>
     <t>MLCC - SMD/SMT 50V 0.1uF X7R 0603 10%</t>
   </si>
   <si>
@@ -94,9 +91,6 @@
     <t>MLCC, X7R, 50V 0603</t>
   </si>
   <si>
-    <t>C5,C7,C9,C10</t>
-  </si>
-  <si>
     <t>MLCC - SMD/SMT 50V 10nF X7R 0603 10%</t>
   </si>
   <si>
@@ -470,12 +464,18 @@
   </si>
   <si>
     <t>DATA 13/12/2023</t>
+  </si>
+  <si>
+    <t>C2,C3,C4,C6,C8,C9,C11,C15,C16</t>
+  </si>
+  <si>
+    <t>C5,C7,C10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1382,11 +1382,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1406,12 +1406,12 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1481,31 +1481,31 @@
         <v>2</v>
       </c>
       <c r="B5" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="E5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="F5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="G5" s="10" t="s">
         <v>20</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>21</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>14</v>
       </c>
       <c r="I5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1513,16 +1513,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>24</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>26</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10" t="s">
@@ -1532,10 +1532,10 @@
         <v>14</v>
       </c>
       <c r="I6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -1546,13 +1546,13 @@
         <v>2</v>
       </c>
       <c r="C7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>27</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>29</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10" t="s">
@@ -1576,26 +1576,26 @@
         <v>1</v>
       </c>
       <c r="C8" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="10" t="s">
         <v>30</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>32</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="J8" s="10" t="s">
         <v>34</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1606,20 +1606,20 @@
         <v>1</v>
       </c>
       <c r="C9" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>37</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>39</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
@@ -1632,26 +1632,26 @@
         <v>1</v>
       </c>
       <c r="C10" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="G10" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="H10" s="10" t="s">
         <v>45</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>47</v>
       </c>
       <c r="I10" s="10"/>
       <c r="J10" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -1662,28 +1662,28 @@
         <v>1</v>
       </c>
       <c r="C11" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="F11" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="G11" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="H11" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>54</v>
-      </c>
       <c r="J11" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -1694,26 +1694,26 @@
         <v>1</v>
       </c>
       <c r="C12" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="G12" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>59</v>
-      </c>
       <c r="H12" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I12" s="10"/>
       <c r="J12" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1724,20 +1724,20 @@
         <v>3</v>
       </c>
       <c r="C13" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>60</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>62</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
@@ -1750,25 +1750,25 @@
         <v>1</v>
       </c>
       <c r="C14" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="F14" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="G14" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="H14" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="I14" s="10" t="s">
         <v>69</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>71</v>
       </c>
       <c r="J14" s="10"/>
     </row>
@@ -1780,28 +1780,28 @@
         <v>5</v>
       </c>
       <c r="C15" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="F15" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="H15" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="G15" s="10" t="s">
+      <c r="I15" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="J15" s="10" t="s">
         <v>76</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="J15" s="10" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1812,23 +1812,23 @@
         <v>1</v>
       </c>
       <c r="C16" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="10" t="s">
         <v>79</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>81</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="I16" s="10" t="s">
         <v>82</v>
-      </c>
-      <c r="H16" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>84</v>
       </c>
       <c r="J16" s="10"/>
     </row>
@@ -1840,13 +1840,13 @@
         <v>12</v>
       </c>
       <c r="C17" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="10" t="s">
         <v>85</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>87</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10" t="s">
@@ -1856,10 +1856,10 @@
         <v>14</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1870,13 +1870,13 @@
         <v>3</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="10" t="s">
@@ -1886,10 +1886,10 @@
         <v>14</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1900,13 +1900,13 @@
         <v>3</v>
       </c>
       <c r="C19" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" s="10" t="s">
         <v>91</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>93</v>
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="10" t="s">
@@ -1916,10 +1916,10 @@
         <v>14</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1930,13 +1930,13 @@
         <v>3</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="10" t="s">
@@ -1946,10 +1946,10 @@
         <v>14</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1960,13 +1960,13 @@
         <v>3</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F21" s="10"/>
       <c r="G21" s="10" t="s">
@@ -1976,10 +1976,10 @@
         <v>14</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1990,13 +1990,13 @@
         <v>1</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="10" t="s">
@@ -2006,10 +2006,10 @@
         <v>14</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2020,13 +2020,13 @@
         <v>2</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10" t="s">
@@ -2036,7 +2036,7 @@
         <v>14</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J23" s="10"/>
     </row>
@@ -2048,20 +2048,20 @@
         <v>15</v>
       </c>
       <c r="C24" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" s="10" t="s">
         <v>104</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>106</v>
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
       <c r="J24" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2072,26 +2072,26 @@
         <v>1</v>
       </c>
       <c r="C25" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E25" s="10" t="s">
         <v>108</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>110</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="I25" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="H25" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="I25" s="10" t="s">
-        <v>113</v>
-      </c>
       <c r="J25" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2102,23 +2102,23 @@
         <v>3</v>
       </c>
       <c r="C26" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="E26" s="10" t="s">
         <v>114</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>116</v>
       </c>
       <c r="F26" s="10"/>
       <c r="G26" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J26" s="10"/>
     </row>
@@ -2130,26 +2130,26 @@
         <v>1</v>
       </c>
       <c r="C27" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="E27" s="10" t="s">
         <v>119</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>121</v>
       </c>
       <c r="F27" s="10"/>
       <c r="G27" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="I27" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="H27" s="10" t="s">
+      <c r="J27" s="10" t="s">
         <v>123</v>
-      </c>
-      <c r="I27" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="J27" s="10" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2160,23 +2160,23 @@
         <v>1</v>
       </c>
       <c r="C28" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E28" s="10" t="s">
         <v>126</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>128</v>
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="I28" s="10" t="s">
         <v>129</v>
-      </c>
-      <c r="H28" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="I28" s="10" t="s">
-        <v>131</v>
       </c>
       <c r="J28" s="10"/>
     </row>
@@ -2188,22 +2188,22 @@
         <v>1</v>
       </c>
       <c r="C29" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="E29" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="F29" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="G29" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="E29" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="F29" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>135</v>
-      </c>
       <c r="H29" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I29" s="10"/>
       <c r="J29" s="10"/>
@@ -2216,26 +2216,26 @@
         <v>1</v>
       </c>
       <c r="C30" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E30" s="10" t="s">
         <v>136</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>138</v>
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I30" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2246,28 +2246,28 @@
         <v>1</v>
       </c>
       <c r="C31" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="E31" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="F31" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="G31" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="H31" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="F31" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="G31" s="10" t="s">
+      <c r="I31" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="H31" s="10" t="s">
+      <c r="J31" s="10" t="s">
         <v>145</v>
-      </c>
-      <c r="I31" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="J31" s="10" t="s">
-        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>